<commit_message>
update plan and NNLS
</commit_message>
<xml_diff>
--- a/schedule/Plan.xlsx
+++ b/schedule/Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\f_PribahsnikF\Documents\GitHub\Masterarbeit\schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\Masterarbeit\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="26">
   <si>
     <t>SEPTEMBER</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Treffen Abnahme NN</t>
+  </si>
+  <si>
+    <t>Abage von Teilergebnissen per Mail</t>
+  </si>
+  <si>
+    <t>Urlaub zum intensiven Schreiben</t>
+  </si>
+  <si>
+    <t>Persönliches Treffen für Feedback/Abschluss der Kapitel</t>
   </si>
 </sst>
 </file>
@@ -141,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +178,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,26 +368,47 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -377,53 +419,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -484,69 +505,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -653,7 +611,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -915,13 +873,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28:R28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
@@ -941,1202 +899,1176 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>43733</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="J2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3">
         <v>43734</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="J3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>43735</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="J4" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="4">
         <v>43736</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4">
         <v>43737</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3">
         <v>43738</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3">
         <v>43739</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="13" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="4">
         <v>43770</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="13" t="s">
+      <c r="J8" s="13"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O8" s="4">
         <v>43800</v>
       </c>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3">
         <v>43740</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="11" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="4">
         <v>43771</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="12" t="s">
+      <c r="J9" s="13"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="O9" s="5">
         <v>43801</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
+      <c r="P9" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>43741</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="11" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="4">
         <v>43772</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="12" t="s">
+      <c r="J10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="O10" s="5">
         <v>43802</v>
       </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3">
         <v>43742</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="16" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="3">
         <v>43773</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="12" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="O11" s="5">
         <v>43803</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="4">
         <v>43743</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="16" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="3">
         <v>43774</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="12" t="s">
+      <c r="J12" s="13"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="8" t="s">
         <v>8</v>
       </c>
       <c r="O12" s="5">
         <v>43804</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4">
         <v>43744</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="16" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="3">
         <v>43775</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="12" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="O13" s="5">
         <v>43805</v>
       </c>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="3">
         <v>43745</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="16" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="3">
         <v>43776</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="11" t="s">
+      <c r="J14" s="13"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="O14" s="4">
         <v>43806</v>
       </c>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="18"/>
+      <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="3">
         <v>43746</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="16" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="3">
         <v>43777</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="11" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O15" s="4">
         <v>43807</v>
       </c>
-      <c r="P15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3">
         <v>43747</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="11" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="4">
         <v>43778</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="12" t="s">
+      <c r="J16" s="13"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="8" t="s">
         <v>5</v>
       </c>
       <c r="O16" s="5">
         <v>43808</v>
       </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="16" t="s">
+      <c r="P16" s="13"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="3">
         <v>43748</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="11" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="4">
         <v>43779</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="12" t="s">
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="O17" s="5">
         <v>43809</v>
       </c>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="16" t="s">
+      <c r="P17" s="13"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3">
         <v>43749</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="17" t="s">
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="6">
         <v>43780</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="12" t="s">
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="8" t="s">
         <v>7</v>
       </c>
       <c r="O18" s="5">
         <v>43810</v>
       </c>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-    </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="11" t="s">
+      <c r="P18" s="13"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="4">
         <v>43750</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="17" t="s">
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="6">
         <v>43781</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="12" t="s">
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="O19" s="5">
         <v>43811</v>
       </c>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="11" t="s">
+      <c r="P19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="4">
         <v>43751</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="16" t="s">
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I20" s="3">
         <v>43782</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="12" t="s">
+      <c r="J20" s="13"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="O20" s="5">
         <v>43812</v>
       </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="16" t="s">
+      <c r="P20" s="13"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3">
         <v>43752</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="16" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I21" s="3">
         <v>43783</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="11" t="s">
+      <c r="J21" s="13"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="O21" s="4">
         <v>43813</v>
       </c>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="16" t="s">
+      <c r="P21" s="13"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="3">
         <v>43753</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="16" t="s">
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="3">
         <v>43784</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="11" t="s">
+      <c r="J22" s="13"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O22" s="4">
         <v>43814</v>
       </c>
-      <c r="P22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-    </row>
-    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="17" t="s">
+      <c r="P22" s="13"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <v>43754</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="11" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="4">
         <v>43785</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="12" t="s">
+      <c r="J23" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="8" t="s">
         <v>5</v>
       </c>
       <c r="O23" s="5">
         <v>43815</v>
       </c>
-      <c r="P23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-    </row>
-    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17" t="s">
+      <c r="P23" s="13"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="6">
         <v>43755</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="11" t="s">
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I24" s="4">
         <v>43786</v>
       </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="12" t="s">
+      <c r="J24" s="13"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="8" t="s">
         <v>6</v>
       </c>
       <c r="O24" s="5">
         <v>43816</v>
       </c>
-      <c r="P24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="17" t="s">
+      <c r="P24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="6">
         <v>43756</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="18" t="s">
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="6">
         <v>43787</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="12" t="s">
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="8" t="s">
         <v>7</v>
       </c>
       <c r="O25" s="5">
         <v>43817</v>
       </c>
-      <c r="P25" s="7" t="s">
+      <c r="P25" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-      <c r="B26" s="11" t="s">
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="4">
         <v>43757</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="17" t="s">
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="6">
         <v>43788</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="12" t="s">
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="O26" s="5">
         <v>43818</v>
       </c>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="11" t="s">
+      <c r="P26" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="4">
         <v>43758</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="16" t="s">
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I27" s="3">
         <v>43789</v>
       </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="12" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="O27" s="5">
         <v>43819</v>
       </c>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-    </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="19" t="s">
+      <c r="P27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="3">
         <v>43759</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="16" t="s">
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I28" s="3">
         <v>43790</v>
       </c>
-      <c r="J28" s="7"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="11" t="s">
+      <c r="J28" s="13"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="O28" s="4">
         <v>43820</v>
       </c>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21"/>
-      <c r="B29" s="16" t="s">
+      <c r="P28" s="13"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="3">
         <v>43760</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="16" t="s">
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="3">
         <v>43791</v>
       </c>
-      <c r="J29" s="7"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="11" t="s">
+      <c r="J29" s="13"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O29" s="4">
         <v>43821</v>
       </c>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-    </row>
-    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
-      <c r="B30" s="17" t="s">
+      <c r="P29" s="13"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>43761</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="11" t="s">
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I30" s="4">
         <v>43792</v>
       </c>
-      <c r="J30" s="7"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="12" t="s">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="8" t="s">
         <v>5</v>
       </c>
       <c r="O30" s="5">
         <v>43822</v>
       </c>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-    </row>
-    <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="17" t="s">
+      <c r="P30" s="13"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+    </row>
+    <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="6">
         <v>43762</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="11" t="s">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I31" s="4">
         <v>43793</v>
       </c>
-      <c r="J31" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="12" t="s">
+      <c r="J31" s="13"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="8" t="s">
         <v>6</v>
       </c>
       <c r="O31" s="5">
         <v>43823</v>
       </c>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-    </row>
-    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="17" t="s">
+      <c r="P31" s="13"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="6">
         <v>43763</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="17" t="s">
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="6">
         <v>43794</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="J32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="11" t="s">
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="7" t="s">
         <v>7</v>
       </c>
       <c r="O32" s="4">
         <v>43824</v>
       </c>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
     </row>
     <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="11" t="s">
+      <c r="A33" s="18"/>
+      <c r="B33" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="4">
         <v>43764</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="17" t="s">
+      <c r="D33" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="6">
         <v>43795</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="J33" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="11" t="s">
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="7" t="s">
         <v>8</v>
       </c>
       <c r="O33" s="4">
         <v>43825</v>
       </c>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="11" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="4">
         <v>43765</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="16" t="s">
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I34" s="3">
         <v>43796</v>
       </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="12" t="s">
+      <c r="J34" s="13"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="8" t="s">
         <v>9</v>
       </c>
       <c r="O34" s="5">
         <v>43826</v>
       </c>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="5">
         <v>43766</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="16" t="s">
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I35" s="3">
         <v>43797</v>
       </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="11" t="s">
+      <c r="J35" s="13"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="7" t="s">
         <v>10</v>
       </c>
       <c r="O35" s="4">
         <v>43827</v>
       </c>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="18"/>
+      <c r="B36" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="3">
         <v>43767</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="16" t="s">
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I36" s="3">
         <v>43798</v>
       </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="11" t="s">
+      <c r="J36" s="13"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O36" s="4">
         <v>43828</v>
       </c>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
     </row>
     <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="21"/>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="3">
         <v>43768</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="11" t="s">
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I37" s="4">
         <v>43799</v>
       </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="12" t="s">
+      <c r="J37" s="13"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="8" t="s">
         <v>5</v>
       </c>
       <c r="O37" s="5">
         <v>43829</v>
       </c>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
     </row>
     <row r="38" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
-      <c r="B38" s="16" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="3">
         <v>43769</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="12" t="s">
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="8" t="s">
         <v>6</v>
       </c>
       <c r="O38" s="5">
         <v>43830</v>
       </c>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="102">
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="P36:R36"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="P27:R27"/>
+  <mergeCells count="104">
+    <mergeCell ref="T31:V31"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="A8:A38"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="G8:G37"/>
+    <mergeCell ref="M8:M38"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
     <mergeCell ref="P28:R28"/>
     <mergeCell ref="P29:R29"/>
     <mergeCell ref="P30:R30"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
@@ -2147,99 +2079,149 @@
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A8:A38"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="G8:G37"/>
-    <mergeCell ref="M8:M38"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="P31:R31"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="expression" dxfId="28" priority="58">
+    <cfRule type="expression" dxfId="16" priority="58">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C38">
-    <cfRule type="cellIs" dxfId="27" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B38">
-    <cfRule type="expression" dxfId="26" priority="53"/>
+    <cfRule type="expression" dxfId="14" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B38">
-    <cfRule type="cellIs" dxfId="25" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="61" operator="equal">
       <formula>"SAD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B38">
-    <cfRule type="expression" dxfId="24" priority="67">
+    <cfRule type="expression" dxfId="12" priority="67">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H35">
-    <cfRule type="expression" dxfId="23" priority="48"/>
+    <cfRule type="expression" dxfId="11" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I37">
-    <cfRule type="expression" dxfId="22" priority="49">
+    <cfRule type="expression" dxfId="10" priority="49">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I37">
-    <cfRule type="cellIs" dxfId="21" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H35">
-    <cfRule type="cellIs" dxfId="20" priority="-1" operator="equal">
-      <formula>"SAD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H35">
-    <cfRule type="expression" dxfId="19" priority="51">
+    <cfRule type="expression" dxfId="8" priority="51">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="expression" dxfId="18" priority="45"/>
+    <cfRule type="expression" dxfId="7" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="cellIs" dxfId="17" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="46" operator="equal">
       <formula>"SAD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="expression" dxfId="16" priority="46">
+    <cfRule type="expression" dxfId="5" priority="68">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N38">
-    <cfRule type="expression" dxfId="7" priority="3"/>
+    <cfRule type="expression" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8:O38">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8:O38">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N38">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="69" operator="equal">
       <formula>"SAD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N38">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>IF(OR(#REF!="SA",#REF!="SO",#REF!=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>